<commit_message>
Pandas (Good), Pandas (Nice)
</commit_message>
<xml_diff>
--- a/pandas/finalised_scores.xlsx
+++ b/pandas/finalised_scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
@@ -492,13 +497,16 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>20.205</v>
+        <v>20.2</v>
       </c>
       <c r="F2" t="n">
         <v>18.96</v>
       </c>
       <c r="G2" t="n">
-        <v>39.165</v>
+        <v>21.25</v>
+      </c>
+      <c r="H2" t="n">
+        <v>60.42</v>
       </c>
     </row>
     <row r="3">
@@ -529,7 +537,10 @@
         <v>17.44</v>
       </c>
       <c r="G3" t="n">
-        <v>30.91</v>
+        <v>18.75</v>
+      </c>
+      <c r="H3" t="n">
+        <v>49.66</v>
       </c>
     </row>
     <row r="4">
@@ -554,13 +565,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>18.366</v>
+        <v>18.37</v>
       </c>
       <c r="F4" t="n">
         <v>15.56</v>
       </c>
       <c r="G4" t="n">
-        <v>33.926</v>
+        <v>43.75</v>
+      </c>
+      <c r="H4" t="n">
+        <v>77.68000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -585,13 +599,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>18.366</v>
+        <v>18.37</v>
       </c>
       <c r="F5" t="n">
         <v>16.36</v>
       </c>
       <c r="G5" t="n">
-        <v>34.726</v>
+        <v>18.75</v>
+      </c>
+      <c r="H5" t="n">
+        <v>53.48</v>
       </c>
     </row>
     <row r="6">
@@ -616,10 +633,17 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>15.306</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+        <v>15.31</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>32.81</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -643,13 +667,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>12.246</v>
+        <v>12.25</v>
       </c>
       <c r="F7" t="n">
-        <v>14.088</v>
+        <v>14.09</v>
       </c>
       <c r="G7" t="n">
-        <v>26.334</v>
+        <v>32.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>58.83</v>
       </c>
     </row>
     <row r="8">
@@ -680,7 +707,10 @@
         <v>16.72</v>
       </c>
       <c r="G8" t="n">
-        <v>33.25</v>
+        <v>31.25</v>
+      </c>
+      <c r="H8" t="n">
+        <v>64.5</v>
       </c>
     </row>
     <row r="9">
@@ -705,13 +735,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>18.981</v>
+        <v>18.98</v>
       </c>
       <c r="F9" t="n">
         <v>16.4</v>
       </c>
       <c r="G9" t="n">
-        <v>35.381</v>
+        <v>43.75</v>
+      </c>
+      <c r="H9" t="n">
+        <v>79.13</v>
       </c>
     </row>
     <row r="10">
@@ -736,13 +769,16 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>15.306</v>
+        <v>15.31</v>
       </c>
       <c r="F10" t="n">
         <v>13.68</v>
       </c>
       <c r="G10" t="n">
-        <v>28.986</v>
+        <v>47.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>76.48999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -767,13 +803,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>17.754</v>
+        <v>17.75</v>
       </c>
       <c r="F11" t="n">
         <v>9.039999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>26.794</v>
+        <v>41.25</v>
+      </c>
+      <c r="H11" t="n">
+        <v>68.04000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -798,13 +837,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>19.593</v>
+        <v>19.59</v>
       </c>
       <c r="F12" t="n">
         <v>16.88</v>
       </c>
       <c r="G12" t="n">
-        <v>36.473</v>
+        <v>32.5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>68.97</v>
       </c>
     </row>
     <row r="13">
@@ -829,13 +871,16 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>26.328</v>
+        <v>26.33</v>
       </c>
       <c r="F13" t="n">
         <v>17</v>
       </c>
       <c r="G13" t="n">
-        <v>43.328</v>
+        <v>50</v>
+      </c>
+      <c r="H13" t="n">
+        <v>93.33</v>
       </c>
     </row>
     <row r="14">
@@ -860,13 +905,16 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>14.082</v>
+        <v>14.08</v>
       </c>
       <c r="F14" t="n">
         <v>16.68</v>
       </c>
       <c r="G14" t="n">
-        <v>30.762</v>
+        <v>41.25</v>
+      </c>
+      <c r="H14" t="n">
+        <v>72.01000000000001</v>
       </c>
     </row>
     <row r="15">
@@ -891,13 +939,16 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>22.041</v>
+        <v>22.04</v>
       </c>
       <c r="F15" t="n">
-        <v>14.128</v>
+        <v>14.13</v>
       </c>
       <c r="G15" t="n">
-        <v>36.169</v>
+        <v>25</v>
+      </c>
+      <c r="H15" t="n">
+        <v>61.17</v>
       </c>
     </row>
     <row r="16">
@@ -921,11 +972,18 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
       <c r="F16" t="n">
         <v>15.72</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>35</v>
+      </c>
+      <c r="H16" t="n">
+        <v>50.72</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -949,13 +1007,16 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>20.817</v>
+        <v>20.82</v>
       </c>
       <c r="F17" t="n">
         <v>14.68</v>
       </c>
       <c r="G17" t="n">
-        <v>35.497</v>
+        <v>20</v>
+      </c>
+      <c r="H17" t="n">
+        <v>55.5</v>
       </c>
     </row>
     <row r="18">
@@ -980,13 +1041,16 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>22.653</v>
+        <v>22.65</v>
       </c>
       <c r="F18" t="n">
-        <v>17.648</v>
+        <v>17.65</v>
       </c>
       <c r="G18" t="n">
-        <v>40.301</v>
+        <v>50</v>
+      </c>
+      <c r="H18" t="n">
+        <v>90.3</v>
       </c>
     </row>
     <row r="19">
@@ -1011,13 +1075,16 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>19.593</v>
+        <v>19.59</v>
       </c>
       <c r="F19" t="n">
         <v>14.68</v>
       </c>
       <c r="G19" t="n">
-        <v>34.273</v>
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>34.27</v>
       </c>
     </row>
     <row r="20">
@@ -1042,13 +1109,16 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>18.981</v>
+        <v>18.98</v>
       </c>
       <c r="F20" t="n">
         <v>15</v>
       </c>
       <c r="G20" t="n">
-        <v>33.981</v>
+        <v>33.75</v>
+      </c>
+      <c r="H20" t="n">
+        <v>67.73</v>
       </c>
     </row>
     <row r="21">
@@ -1073,13 +1143,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>15.306</v>
+        <v>15.31</v>
       </c>
       <c r="F21" t="n">
-        <v>16.016</v>
+        <v>16.02</v>
       </c>
       <c r="G21" t="n">
-        <v>31.322</v>
+        <v>43.75</v>
+      </c>
+      <c r="H21" t="n">
+        <v>75.06999999999999</v>
       </c>
     </row>
     <row r="22">
@@ -1104,10 +1177,17 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>12.858</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+        <v>12.86</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>46.25</v>
+      </c>
+      <c r="H22" t="n">
+        <v>59.11</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1131,13 +1211,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>23.877</v>
+        <v>23.88</v>
       </c>
       <c r="F23" t="n">
-        <v>17.648</v>
+        <v>17.65</v>
       </c>
       <c r="G23" t="n">
-        <v>41.525</v>
+        <v>32.5</v>
+      </c>
+      <c r="H23" t="n">
+        <v>74.03</v>
       </c>
     </row>
     <row r="24">
@@ -1162,13 +1245,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>15.918</v>
+        <v>15.92</v>
       </c>
       <c r="F24" t="n">
         <v>14.36</v>
       </c>
       <c r="G24" t="n">
-        <v>30.278</v>
+        <v>41.25</v>
+      </c>
+      <c r="H24" t="n">
+        <v>71.53</v>
       </c>
     </row>
     <row r="25">
@@ -1193,13 +1279,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>22.041</v>
+        <v>22.04</v>
       </c>
       <c r="F25" t="n">
         <v>16.88</v>
       </c>
       <c r="G25" t="n">
-        <v>38.921</v>
+        <v>22.5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>61.42</v>
       </c>
     </row>
     <row r="26">
@@ -1224,13 +1313,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>19.593</v>
+        <v>19.59</v>
       </c>
       <c r="F26" t="n">
         <v>14.36</v>
       </c>
       <c r="G26" t="n">
-        <v>33.953</v>
+        <v>30</v>
+      </c>
+      <c r="H26" t="n">
+        <v>63.95</v>
       </c>
     </row>
     <row r="27">
@@ -1255,13 +1347,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>12.858</v>
+        <v>12.86</v>
       </c>
       <c r="F27" t="n">
         <v>18.08</v>
       </c>
       <c r="G27" t="n">
-        <v>30.938</v>
+        <v>47.5</v>
+      </c>
+      <c r="H27" t="n">
+        <v>78.44</v>
       </c>
     </row>
     <row r="28">
@@ -1286,13 +1381,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>23.265</v>
+        <v>23.26</v>
       </c>
       <c r="F28" t="n">
         <v>14.36</v>
       </c>
       <c r="G28" t="n">
-        <v>37.625</v>
+        <v>31.25</v>
+      </c>
+      <c r="H28" t="n">
+        <v>68.88</v>
       </c>
     </row>
     <row r="29">
@@ -1317,13 +1415,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>20.817</v>
+        <v>20.82</v>
       </c>
       <c r="F29" t="n">
         <v>15.92</v>
       </c>
       <c r="G29" t="n">
-        <v>36.737</v>
+        <v>16.25</v>
+      </c>
+      <c r="H29" t="n">
+        <v>52.99</v>
       </c>
     </row>
     <row r="30">
@@ -1347,9 +1448,18 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1373,13 +1483,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>18.366</v>
+        <v>18.37</v>
       </c>
       <c r="F31" t="n">
         <v>11</v>
       </c>
       <c r="G31" t="n">
-        <v>29.366</v>
+        <v>28.75</v>
+      </c>
+      <c r="H31" t="n">
+        <v>58.12</v>
       </c>
     </row>
     <row r="32">
@@ -1404,13 +1517,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>18.366</v>
+        <v>18.37</v>
       </c>
       <c r="F32" t="n">
         <v>16.8</v>
       </c>
       <c r="G32" t="n">
-        <v>35.166</v>
+        <v>36.25</v>
+      </c>
+      <c r="H32" t="n">
+        <v>71.42</v>
       </c>
     </row>
     <row r="33">
@@ -1435,13 +1551,16 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>22.653</v>
+        <v>22.65</v>
       </c>
       <c r="F33" t="n">
         <v>17.76</v>
       </c>
       <c r="G33" t="n">
-        <v>40.413</v>
+        <v>16.25</v>
+      </c>
+      <c r="H33" t="n">
+        <v>56.66</v>
       </c>
     </row>
     <row r="34">
@@ -1472,6 +1591,9 @@
         <v>10.28</v>
       </c>
       <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
         <v>26.81</v>
       </c>
     </row>
@@ -1497,13 +1619,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>17.754</v>
+        <v>17.75</v>
       </c>
       <c r="F35" t="n">
         <v>15.04</v>
       </c>
       <c r="G35" t="n">
-        <v>32.794</v>
+        <v>25</v>
+      </c>
+      <c r="H35" t="n">
+        <v>57.79</v>
       </c>
     </row>
     <row r="36">
@@ -1528,13 +1653,16 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>20.817</v>
+        <v>20.82</v>
       </c>
       <c r="F36" t="n">
-        <v>13.816</v>
+        <v>13.82</v>
       </c>
       <c r="G36" t="n">
-        <v>34.633</v>
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>34.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>